<commit_message>
more day20 analysis - possibly the answer
</commit_message>
<xml_diff>
--- a/Runner/ManualAnalysis/Day20.xlsx
+++ b/Runner/ManualAnalysis/Day20.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="88">
   <si>
     <t>^ENW$</t>
   </si>
@@ -221,10 +221,76 @@
     <t>{2}</t>
   </si>
   <si>
-    <t>(nnn|eee|www|sss)(n|s)eee</t>
-  </si>
-  <si>
-    <t>nnn(eee|www)sss</t>
+    <t>A</t>
+  </si>
+  <si>
+    <t>ESSWWN</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>^A(B|C(D(E|)F|G(H|I)))$</t>
+  </si>
+  <si>
+    <t>currentRoutes</t>
+  </si>
+  <si>
+    <t>wholeTermRoutes</t>
+  </si>
+  <si>
+    <t>| = copy currentRoutes to wholeTermRoutes</t>
+  </si>
+  <si>
+    <t>)=return currentRoutes union wholeTermRoutes</t>
+  </si>
+  <si>
+    <t>GH,GI</t>
+  </si>
+  <si>
+    <t>{empty}</t>
+  </si>
+  <si>
+    <t>( = call recursive, add returned routes to each of current routes to current routes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unless first is empty, in which case add returned routes to each of current routes </t>
+  </si>
+  <si>
+    <t>(except empty) to each of wholeTermRoutes</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>DF</t>
+  </si>
+  <si>
+    <t>DE,DF</t>
+  </si>
+  <si>
+    <t>CGH,CGI,CDE,CDF</t>
+  </si>
+  <si>
+    <t>ACGH,ACGI,ACDE,ACDF,AB</t>
   </si>
 </sst>
 </file>
@@ -246,7 +312,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -259,8 +325,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -268,17 +340,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,7 +640,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1244,7 +1333,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -1455,23 +1544,479 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:A11"/>
+  <dimension ref="A3:J36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="11" spans="1:1">
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>65</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G22" s="5"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I24" s="5"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J26" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G27" s="5"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="I31" s="5"/>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>